<commit_message>
Added 1kB EEPROM chip to V0.2.2 board
</commit_message>
<xml_diff>
--- a/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.2/BOM NOT UPDATED.xlsx
+++ b/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.2/BOM NOT UPDATED.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-440" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tilty Duo BT" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="135">
   <si>
     <t>Part</t>
   </si>
@@ -388,9 +388,6 @@
     <t>QFN/Leadless</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
@@ -425,6 +422,12 @@
   </si>
   <si>
     <t>160-1415-1-ND</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>24</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -1430,22 +1433,22 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
         <v>130</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>131</v>
       </c>
       <c r="G11" s="2">
         <v>0.35</v>
@@ -1466,7 +1469,7 @@
         <v>46</v>
       </c>
       <c r="M11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N11" s="11">
         <v>0.39900000000000002</v>
@@ -1484,7 +1487,7 @@
         <v>66</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C12" t="s">
         <v>67</v>
@@ -1496,7 +1499,7 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G12" s="2">
         <v>0.34</v>
@@ -1523,7 +1526,7 @@
         <v>64</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C13" t="s">
         <v>65</v>
@@ -1535,7 +1538,7 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G13" s="2">
         <v>0.34</v>
@@ -2416,7 +2419,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="B11:B12 B14:B24" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -2844,7 +2846,7 @@
         <v>64</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
         <v>65</v>
@@ -2856,7 +2858,7 @@
         <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G11" s="2">
         <v>0.34</v>
@@ -3726,8 +3728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:Q15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4229,22 +4231,22 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
         <v>130</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" t="s">
-        <v>131</v>
       </c>
       <c r="G13" s="2">
         <v>0.35</v>
@@ -4265,7 +4267,7 @@
         <v>46</v>
       </c>
       <c r="M13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N13" s="11">
         <v>0.39900000000000002</v>
@@ -4283,7 +4285,7 @@
         <v>66</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C14" t="s">
         <v>67</v>
@@ -4295,7 +4297,7 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G14" s="2">
         <v>0.34</v>
@@ -4322,7 +4324,7 @@
         <v>64</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C15" t="s">
         <v>65</v>
@@ -4334,7 +4336,7 @@
         <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G15" s="2">
         <v>0.34</v>
@@ -4964,7 +4966,7 @@
         <v>116</v>
       </c>
       <c r="B32" s="29">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -4972,7 +4974,7 @@
         <v>117</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -4980,7 +4982,7 @@
         <v>118</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D34" s="5"/>
       <c r="G34" s="2"/>
@@ -4995,7 +4997,7 @@
         <v>119</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="D35" s="5"/>
       <c r="G35" s="2"/>
@@ -5010,7 +5012,7 @@
         <v>120</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="2"/>
@@ -5277,9 +5279,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="B17:B28 B33:B36" numberStoredAsText="1"/>
+    <ignoredError sqref="B17:B28 B34 B36" numberStoredAsText="1"/>
     <ignoredError sqref="Q26 Q20 Q10 Q4" formula="1"/>
     <ignoredError sqref="Q30" emptyCellReference="1"/>
   </ignoredErrors>
@@ -5806,7 +5807,7 @@
         <v>64</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C13" t="s">
         <v>65</v>
@@ -5818,7 +5819,7 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G13" s="2">
         <v>0.34</v>
@@ -6701,10 +6702,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="28" t="s">
         <v>124</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -6773,7 +6774,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:6">

</xml_diff>

<commit_message>
Software and Hardware update
</commit_message>
<xml_diff>
--- a/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.2/BOM NOT UPDATED.xlsx
+++ b/Tilty Hardware/Board Files/Tilty Duo:Quad/V0.2.2/BOM NOT UPDATED.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23480" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tilty Duo BT" sheetId="1" r:id="rId1"/>
@@ -3728,8 +3728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6689,8 +6689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>